<commit_message>
Updated for loading screens.
</commit_message>
<xml_diff>
--- a/Ads_Crawler.xlsx
+++ b/Ads_Crawler.xlsx
@@ -10,6 +10,8 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$85</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$85</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$85</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -293,7 +295,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -307,14 +309,6 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -335,18 +329,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -656,7 +647,7 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -918,7 +909,7 @@
         <f>A21&amp;"/ads.txt"</f>
         <v/>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>5</v>
       </c>
     </row>
@@ -943,7 +934,7 @@
         <v/>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1014,7 +1005,7 @@
         <f>A29&amp;"/ads.txt"</f>
         <v/>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1206,7 +1197,7 @@
         <f>A45&amp;"/ads.txt"</f>
         <v/>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1242,7 +1233,9 @@
         <f>A48&amp;"/ads.txt"</f>
         <v/>
       </c>
-      <c r="C48" s="2" t="n"/>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
@@ -1252,6 +1245,9 @@
         <f>A49&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
@@ -1261,6 +1257,9 @@
         <f>A50&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
@@ -1270,6 +1269,9 @@
         <f>A51&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
@@ -1279,6 +1281,9 @@
         <f>A52&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
@@ -1288,6 +1293,9 @@
         <f>A53&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
@@ -1297,6 +1305,9 @@
         <f>A54&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
@@ -1306,6 +1317,9 @@
         <f>A55&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
@@ -1315,6 +1329,9 @@
         <f>A56&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
@@ -1324,6 +1341,9 @@
         <f>A57&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
@@ -1333,6 +1353,9 @@
         <f>A58&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
@@ -1342,6 +1365,9 @@
         <f>A59&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
@@ -1351,6 +1377,9 @@
         <f>A60&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
@@ -1360,6 +1389,9 @@
         <f>A61&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
@@ -1369,6 +1401,9 @@
         <f>A62&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
@@ -1378,6 +1413,9 @@
         <f>A63&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
@@ -1387,6 +1425,9 @@
         <f>A64&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
@@ -1396,6 +1437,9 @@
         <f>A65&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
@@ -1405,6 +1449,9 @@
         <f>A66&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
@@ -1414,6 +1461,9 @@
         <f>A67&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
@@ -1423,6 +1473,9 @@
         <f>A68&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
@@ -1432,6 +1485,9 @@
         <f>A69&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
@@ -1441,6 +1497,9 @@
         <f>A70&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
@@ -1450,6 +1509,9 @@
         <f>A71&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
@@ -1459,6 +1521,9 @@
         <f>A72&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
@@ -1468,6 +1533,9 @@
         <f>A73&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
@@ -1477,6 +1545,9 @@
         <f>A74&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
@@ -1486,6 +1557,9 @@
         <f>A75&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
@@ -1495,6 +1569,9 @@
         <f>A76&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
@@ -1504,6 +1581,9 @@
         <f>A77&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
@@ -1513,6 +1593,9 @@
         <f>A78&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
@@ -1522,6 +1605,9 @@
         <f>A79&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
@@ -1531,6 +1617,9 @@
         <f>A80&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
@@ -1540,6 +1629,9 @@
         <f>A81&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
@@ -1549,6 +1641,9 @@
         <f>A82&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
@@ -1558,6 +1653,9 @@
         <f>A83&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
@@ -1567,6 +1665,9 @@
         <f>A84&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C84" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
@@ -1576,8 +1677,12 @@
         <f>A85&amp;"/ads.txt"</f>
         <v/>
       </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F85"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated search_str to search_set
</commit_message>
<xml_diff>
--- a/Ads_Crawler.xlsx
+++ b/Ads_Crawler.xlsx
@@ -9,53 +9,89 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$85</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$85</definedName>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$F$85</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
   <si>
     <t>Domain/Sites</t>
   </si>
   <si>
-    <t>ads.txt</t>
-  </si>
-  <si>
-    <t>Search for</t>
+    <t>Found</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Search for:</t>
+  </si>
+  <si>
+    <t>diario.mx</t>
+  </si>
+  <si>
+    <t>pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx</t>
   </si>
   <si>
     <t>ey5io-qyxzx</t>
   </si>
   <si>
-    <t>diario.mx</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>elmundo.es</t>
   </si>
   <si>
-    <t>No</t>
+    <t>pub-4769180667814197, pub-4769180667814197, pub-4769180667814197, pub-4769180667814197, pub-4769180667814197, pub-4769180667814197</t>
+  </si>
+  <si>
+    <t>ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx</t>
+  </si>
+  <si>
+    <t>pub-4769180667814197</t>
   </si>
   <si>
     <t>elsalvador.com</t>
   </si>
   <si>
+    <t>pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx</t>
+  </si>
+  <si>
     <t>tn.com.ar</t>
   </si>
   <si>
+    <t>pub-4769180667814197, pub-4769180667814197, pub-4769180667814197</t>
+  </si>
+  <si>
+    <t>ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx</t>
+  </si>
+  <si>
     <t>ovaciondigital.com.uy</t>
   </si>
   <si>
+    <t>pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx</t>
+  </si>
+  <si>
     <t>lavanguardia.com</t>
   </si>
   <si>
+    <t>pub-4769180667814197, pub-4769180667814197</t>
+  </si>
+  <si>
+    <t>ey5io-qyxzx, ey5io-qyxzx</t>
+  </si>
+  <si>
     <t>esto.com.mx</t>
   </si>
   <si>
@@ -68,6 +104,9 @@
     <t>elnacional.com</t>
   </si>
   <si>
+    <t>pub-4769180667814197, ey5io-qyxzx</t>
+  </si>
+  <si>
     <t>americatv.com.pe</t>
   </si>
   <si>
@@ -288,6 +327,21 @@
   </si>
   <si>
     <t>peru21.pe</t>
+  </si>
+  <si>
+    <t>pub-4769180667814197, pub-4769180667814197, pub-4769180667814197, pub-4769180667814197, pub-4769180667814197, pub-4769180667814197, pub-4769180667814197</t>
+  </si>
+  <si>
+    <t>ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx</t>
+  </si>
+  <si>
+    <t>pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx, pub-4769180667814197, ey5io-qyxzx</t>
+  </si>
+  <si>
+    <t>pub-4769180667814197, pub-4769180667814197, pub-4769180667814197, pub-4769180667814197</t>
+  </si>
+  <si>
+    <t>ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx, ey5io-qyxzx</t>
   </si>
 </sst>
 </file>
@@ -647,1042 +701,518 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="26.5"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="33"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="8.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="10"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="10"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="70.83203125"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="39.83203125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="8.1640625"/>
+    <col customWidth="1" max="5" min="5" width="8.1640625"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="20.33203125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <f>A2&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <f>A3&amp;"/ads.txt"</f>
-        <v/>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>102</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <f>A4&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <f>A5&amp;"/ads.txt"</f>
-        <v/>
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <f>A6&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <f>A7&amp;"/ads.txt"</f>
-        <v/>
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <f>A8&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <f>A9&amp;"/ads.txt"</f>
-        <v/>
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <f>A10&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <f>A11&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <f>A12&amp;"/ads.txt"</f>
-        <v/>
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <f>A13&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <f>A14&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <f>A15&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
-        <f>A16&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <f>A17&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <f>A18&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <f>A19&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
-        <f>A20&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <f>A21&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22">
-        <f>A22&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23">
-        <f>A23&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24">
-        <f>A24&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25">
-        <f>A25&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26">
-        <f>A26&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27">
-        <f>A27&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28">
-        <f>A28&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29">
-        <f>A29&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30">
-        <f>A30&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31">
-        <f>A31&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32">
-        <f>A32&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33">
-        <f>A33&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34">
-        <f>A34&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35">
-        <f>A35&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36">
-        <f>A36&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37">
-        <f>A37&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38">
-        <f>A38&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39">
-        <f>A39&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40">
-        <f>A40&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41">
-        <f>A41&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C41" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42">
-        <f>A42&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C42" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43">
-        <f>A43&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44">
-        <f>A44&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45">
-        <f>A45&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46">
-        <f>A46&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C46" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47">
-        <f>A47&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C47" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48">
-        <f>A48&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C48" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49">
-        <f>A49&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50">
-        <f>A50&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C50" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51">
-        <f>A51&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C51" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52">
-        <f>A52&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C52" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53">
-        <f>A53&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C53" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54">
-        <f>A54&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C54" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55">
-        <f>A55&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56">
-        <f>A56&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C56" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57">
-        <f>A57&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58">
-        <f>A58&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>63</v>
-      </c>
-      <c r="B59">
-        <f>A59&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C59" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60">
-        <f>A60&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C60" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61">
-        <f>A61&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C61" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62">
-        <f>A62&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C62" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63">
-        <f>A63&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C63" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64">
-        <f>A64&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C64" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65">
-        <f>A65&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C65" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66">
-        <f>A66&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C66" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67">
-        <f>A67&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C67" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>72</v>
-      </c>
-      <c r="B68">
-        <f>A68&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C68" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>73</v>
-      </c>
-      <c r="B69">
-        <f>A69&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C69" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>74</v>
-      </c>
-      <c r="B70">
-        <f>A70&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C70" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>75</v>
-      </c>
-      <c r="B71">
-        <f>A71&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C71" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>76</v>
-      </c>
-      <c r="B72">
-        <f>A72&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C72" t="s">
-        <v>5</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>77</v>
-      </c>
-      <c r="B73">
-        <f>A73&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C73" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>78</v>
-      </c>
-      <c r="B74">
-        <f>A74&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C74" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>79</v>
-      </c>
-      <c r="B75">
-        <f>A75&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C75" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>80</v>
-      </c>
-      <c r="B76">
-        <f>A76&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C76" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>81</v>
-      </c>
-      <c r="B77">
-        <f>A77&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C77" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78">
-        <f>A78&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C78" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>83</v>
-      </c>
-      <c r="B79">
-        <f>A79&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C79" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80">
-        <f>A80&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C80" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81">
-        <f>A81&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C81" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>86</v>
-      </c>
-      <c r="B82">
-        <f>A82&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C82" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>87</v>
-      </c>
-      <c r="B83">
-        <f>A83&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C83" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84">
-        <f>A84&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C84" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>89</v>
-      </c>
-      <c r="B85">
-        <f>A85&amp;"/ads.txt"</f>
-        <v/>
-      </c>
-      <c r="C85" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F85"/>
+  <autoFilter ref="A1:D1"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified open code to accounts for BadStatusLine error.
</commit_message>
<xml_diff>
--- a/Ads_Crawler.xlsx
+++ b/Ads_Crawler.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javieravitia/Desktop/HCode/Ads_Crawler/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{887A8D5B-46A6-CD4C-8DEC-E3EBA0E4ABDC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="32040" yWindow="1860" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$307</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$307</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="498">
   <si>
     <t>Domain/Sites</t>
   </si>
@@ -660,7 +667,7 @@
     <t>lapaginamillionaria.com</t>
   </si>
   <si>
-    <t xml:space="preserve">LaPaginaMillonaria.com </t>
+    <t>LaPaginaMillonaria.com </t>
   </si>
   <si>
     <t>lapatilla.com</t>
@@ -1101,6 +1108,9 @@
     <t>137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 1356, 762769, 156212, 10440, 762737, 1360, 101557, 18008, 538959099</t>
   </si>
   <si>
+    <t>Verify URL manually.</t>
+  </si>
+  <si>
     <t>137711, 185362, 95838, 232757, 247572, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 15777, 184081, 1360, 101557, 538959099</t>
   </si>
   <si>
@@ -1141,33 +1151,398 @@
   </si>
   <si>
     <t>82069, pub-1956856209985681, 493, 539924617, 17960, 527, 156700, 1fe16a48, 762769, 10440, 762737, 1360, 18008</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 8790, 15777, 156500, 184081, pub-7995104076770938, 1360, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>82069, pub-1956856209985681, 247572, 493, 527, 1fe16a48, 1356, 762769, 10440, 762737, 18008</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 156212, 8790, 15777, 10440, 762737, 156500, 184081, pub-7995104076770938, 1360, 101557, 18008, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 15777, 184081, 101557, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 1356, 762769, 8790, 10440, 762737, 156500, pub-7995104076770938, 1360, 18008, 16156</t>
+  </si>
+  <si>
+    <t>8035, 13894, pub-4769180667814197, 4aa37fe0, 5322, 8790, 156500, pub-7995104076770938, 101557, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 282, 11645, ey5io-qyxzx, 20535, 1fe16a48, 1356, 120, 762769, 156212, 15777, 10440, 762737, 184081, 1360, 18008, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 15777, 184081, pub-7995104076770938, 101557, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 1356, 762769, 8790, 10440, 762737, 156500, 1360, 18008, 16156</t>
+  </si>
+  <si>
+    <t>95838, 232757, 282, ey5io-qyxzx, 4aa37fe0, 15777, 148395</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, 11645, pub-4769180667814197, 20535, 1fe16a48, 1356, 120, 762769, 5322, 156212, 8790, 10440, 762737, 156500, 184081, pub-7995104076770938, 1360, 101557, 18008, 538959099, 16156</t>
+  </si>
+  <si>
+    <t>137711, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 5322, 156212, 8790, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>13894, 282, pub-4769180667814197, 148395</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 156212, 8790, 15777, 10440, 762737, 156500, 184081, pub-7995104076770938, 1360, 101557, 18008, 538959099, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 8790, 15777, 184081, pub-7995104076770938, 101557, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 1356, 762769, 10440, 762737, 156500, 1360, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 13894, 282, pub-4769180667814197, 1356, 156212, 8790, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 8790, 15777, 156500, 184081, pub-7995104076770938, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 1fe16a48, 1356, 762769, 10440, 762737, 1360, 18008</t>
+  </si>
+  <si>
+    <t>8790, pub-7995104076770938</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 156212, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 13894, 282, 11645, pub-4769180667814197, 1356, 120, 156212, 8790, 184081, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 762769, 5322, 15777, 10440, 762737, 156500, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>185362, 95838, 232757, 13894, pub-4769180667814197, 1356, 8790, pub-7995104076770938</t>
+  </si>
+  <si>
+    <t>8035, 137711, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 282, 11645, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 156212, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 1356, 156212, 8790, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 232757, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 1356, 120, 156212, 8790, 184081, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 4aa37fe0, 1fe16a48, 762769, 5322, 15777, 10440, 762737, 156500, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 11645, 1356, 156212, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 8790, 15777, 10440, 762737, 156500, 184081, pub-7995104076770938, 1360, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 156500, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 247572, 493, 13894, 539924617, 17960, 527, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 156212, 8790, 15777, 10440, 762737, 184081, pub-7995104076770938, 1360, 101557, 18008, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 8790, 15777, 184081, pub-7995104076770938, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>8035, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 1fe16a48, 762769, 10440, 762737, 156500, 1360, 101557, 18008</t>
+  </si>
+  <si>
+    <t>13894, 282, pub-4769180667814197, 8790, pub-7995104076770938, 148395</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 156212, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 538959099, 16156</t>
+  </si>
+  <si>
+    <t>137711, 13894, 539924617, 17960, 156700, 11645, pub-4769180667814197, 4aa37fe0, 120, 5322, 156212, 15777, 184081, pub-7995104076770938, 1360, 101557, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 527, 282, ey5io-qyxzx, 20535, 1fe16a48, 1356, 762769, 8790, 10440, 762737, 156500, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 8790, 15777, 184081, pub-7995104076770938, 101557, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 762769, 10440, 762737, 156500, 1360, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 232757, 247572, 13894, 539924617, 17960, 156700, 11645, pub-4769180667814197, 1356, 156212, 1360, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 82069, pub-1956856209985681, 493, 527, 282, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 8790, 15777, 10440, 762737, 156500, 184081, pub-7995104076770938, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 15777, 184081, 101557, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 1fe16a48, 762769, 8790, 10440, 762737, 156500, pub-7995104076770938, 1360, 18008, 16156</t>
+  </si>
+  <si>
+    <t>8035, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 1356, 8790, 156500, pub-7995104076770938, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 156212, 15777, 10440, 762737, 184081, 1360, 101557, 18008, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>82069, pub-1956856209985681, 247572, 493, 527, 1356, 762769, 762737, 18008</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 5322, 156212, 8790, 15777, 10440, 156500, 184081, pub-7995104076770938, 1360, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 8790, 15777, 156500, 184081, pub-7995104076770938, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 762769, 10440, 762737, 1360, 18008</t>
+  </si>
+  <si>
+    <t>8035, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 8790, 156500, 184081, pub-7995104076770938, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 1356, 762769, 156212, 15777, 10440, 762737, 1360, 101557, 18008, 538959099</t>
+  </si>
+  <si>
+    <t>137711, 232757, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 1356, 120, 156212, 8790, 184081, pub-7995104076770938, 1360, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 82069, pub-1956856209985681, 247572, 493, 527, 4aa37fe0, 1fe16a48, 762769, 5322, 15777, 10440, 762737, 156500, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 282, 11645, pub-4769180667814197, 1356, 120, 156212, 8790, 184081, pub-7995104076770938, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 762769, 5322, 15777, 10440, 762737, 156500, 1360, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>8035, 137711, 13894, 11645, pub-4769180667814197, 156212, 8790, 156500, 538959099, 16156</t>
+  </si>
+  <si>
+    <t>185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 282, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 15777, 10440, 762737, 184081, pub-7995104076770938, 1360, 101557, 18008, 148395</t>
+  </si>
+  <si>
+    <t>137711, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, 1356, 120, 156212, 8790, 184081, pub-7995104076770938, 1360, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 527, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 762769, 5322, 15777, 10440, 762737, 156500, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>185362, 95838, 232757, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 8790, 15777, 184081, pub-7995104076770938, 101557, 148395</t>
+  </si>
+  <si>
+    <t>8035, 137711, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 1356, 762769, 156212, 10440, 762737, 156500, 1360, 18008, 538959099, 16156</t>
+  </si>
+  <si>
+    <t>137711, pub-1956856209985681, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 120, 156212, 8790, 184081, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, 247572, 493, 13894, 539924617, 17960, 527, 156700, 4aa37fe0, 1fe16a48, 1356, 762769, 5322, 15777, 10440, 762737, 156500, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 8790, 15777, 184081, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 1fe16a48, 762769, 10440, 762737, 156500, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 247572, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 15777, 184081, pub-7995104076770938, 101557, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 493, 539924617, 17960, 527, 156700, 1fe16a48, 762769, 8790, 10440, 762737, 156500, 1360, 18008, 16156</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 8790, 15777, 156500, 184081, pub-7995104076770938, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 1fe16a48, 1356, 762769, 10440, 762737, 1360, 18008</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 247572, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 15777, 184081, 101557, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 493, 539924617, 17960, 527, 156700, 1fe16a48, 762769, 8790, 10440, 762737, 156500, pub-7995104076770938, 1360, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 8790, 15777, 184081, pub-7995104076770938, 1360, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 232757, 82069, pub-1956856209985681, 247572, 493, 527, 1fe16a48, 762769, 10440, 762737, 156500, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 232757, 247572, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, 1356, 156212, 8790, pub-7995104076770938, 1360, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 82069, pub-1956856209985681, 493, 527, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 13894, 282, 11645, pub-4769180667814197, 1356, 156212, 8790, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 156212, 8790, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 11645, 156212, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 8790, 15777, 10440, 762737, 156500, 184081, pub-7995104076770938, 1360, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 247572, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 1356, 156212, 8790, pub-7995104076770938, 1360, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 493, 527, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 13894, 156700, 282, 11645, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 8790, 15777, 156500, 184081, pub-7995104076770938, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, pub-4769180667814197, 1fe16a48, 1356, 762769, 10440, 762737, 1360, 18008</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 762769, 5322, 156212, 8790, 15777, 10440, 762737, 156500, 184081, pub-7995104076770938, 1360, 101557, 18008, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 282, 11645, pub-4769180667814197, 120, 156212, 8790, 184081, pub-7995104076770938, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 762769, 5322, 15777, 10440, 762737, 156500, 1360, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 282, 11645, pub-4769180667814197, 1356, 120, 156212, 184081, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 762769, 5322, 8790, 15777, 10440, 762737, 156500, pub-7995104076770938, 1360, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>137711, 232757, 247572, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 1356, 156212, 8790, pub-7995104076770938, 1360, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 82069, pub-1956856209985681, 493, 527, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 247572, 13894, pub-4769180667814197, 156212, 8790, pub-7995104076770938</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 493, 539924617, 17960, 527, 156700, 282, 11645, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>232757, 13894, pub-4769180667814197, 8790, pub-7995104076770938</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 282, 11645, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 156212, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>232757, 82069, pub-1956856209985681, 247572, 13894, 527, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 762769, 5322, 8790, 762737, 184081, pub-7995104076770938, 18008, 148395</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 493, 539924617, 17960, 156700, 11645, 1fe16a48, 156212, 15777, 10440, 156500, 1360, 101557, 538959099, 16156</t>
+  </si>
+  <si>
+    <t>137711, 82069, pub-1956856209985681, 282, 11645, pub-4769180667814197, 1356, 120, 156212, 8790, 184081, pub-7995104076770938, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 247572, 493, 13894, 539924617, 17960, 527, 156700, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 762769, 5322, 15777, 10440, 762737, 156500, 1360, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>8035, 156500, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 539924617, 17960, 527, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 1356, 120, 762769, 5322, 156212, 8790, 15777, 10440, 762737, 184081, pub-7995104076770938, 1360, 101557, 18008, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 13894, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 8790, 15777, 156500, 184081, pub-7995104076770938, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 1fe16a48, 762769, 10440, 762737, 1360, 18008</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 8790, 15777, 156500, 184081, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 1fe16a48, 1356, 762769, 10440, 762737, pub-7995104076770938, 1360, 18008</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 13894, 539924617, 17960, 156700, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 120, 5322, 156212, 8790, 15777, 184081, pub-7995104076770938, 1360, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 232757, 82069, pub-1956856209985681, 247572, 493, 527, 1fe16a48, 1356, 762769, 10440, 762737, 156500, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 247572, 539924617, 17960, 156700, 11645, 1356, 156212, 1360, 538959099</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 493, 13894, 527, 282, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 8790, 15777, 10440, 762737, 156500, 184081, pub-7995104076770938, 101557, 18008, 148395, 16156</t>
+  </si>
+  <si>
+    <t>8035, 137711, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 13894, 527, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 762769, 5322, 156212, 8790, 15777, 762737, 156500, 184081, pub-7995104076770938, 101557, 18008, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>539924617, 17960, 156700, 1fe16a48, 10440, 1360</t>
+  </si>
+  <si>
+    <t>137711, 13894, 282, pub-4769180667814197, ey5io-qyxzx, 1356, 156212, 8790, pub-7995104076770938, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 185362, 95838, 232757, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 11645, 20535, 4aa37fe0, 1fe16a48, 120, 762769, 5322, 15777, 10440, 762737, 156500, 184081, 1360, 101557, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 247572, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 8790, 15777, 184081, pub-7995104076770938, 101557, 538959099, 148395</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 493, 539924617, 17960, 527, 156700, 1fe16a48, 762769, 10440, 762737, 156500, 1360, 18008, 16156</t>
+  </si>
+  <si>
+    <t>137711, 185362, 95838, 232757, 13894, 282, 11645, pub-4769180667814197, ey5io-qyxzx, 20535, 4aa37fe0, 1356, 120, 5322, 156212, 8790, 15777, 184081, pub-7995104076770938, 101557, 538959099, 148395, 16156</t>
+  </si>
+  <si>
+    <t>8035, 82069, pub-1956856209985681, 247572, 493, 539924617, 17960, 527, 156700, 1fe16a48, 762769, 10440, 762737, 156500, 1360, 18008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1183,23 +1558,32 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1499,29 +1883,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F307"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="4" width="26.5"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="4" width="70.83203125"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="4" width="255.83203125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="4" width="8.1640625"/>
-    <col customWidth="1" max="5" min="5" style="4" width="8.1640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="3" width="21.5"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="4" width="20.83203125"/>
+    <col min="1" max="1" width="25.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1534,12 +1913,12 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="n"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1553,7 +1932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1564,7 +1943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1575,7 +1954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1586,7 +1965,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1600,7 +1979,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1614,7 +1993,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1628,7 +2007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1642,102 +2021,102 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>352</v>
+      <c r="D10" t="s">
+        <v>361</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C11" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C12" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C13" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C14" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C15" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C16" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1748,1560 +2127,3013 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C18" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C19" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
+      <c r="C20" t="s">
+        <v>352</v>
+      </c>
       <c r="F20" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
+      <c r="B21" t="s">
+        <v>376</v>
+      </c>
+      <c r="C21" t="s">
+        <v>377</v>
+      </c>
       <c r="F21" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>43</v>
       </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>378</v>
+      </c>
       <c r="F22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>45</v>
       </c>
+      <c r="B23" t="s">
+        <v>359</v>
+      </c>
+      <c r="C23" t="s">
+        <v>360</v>
+      </c>
       <c r="F23" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>47</v>
       </c>
+      <c r="B24" t="s">
+        <v>379</v>
+      </c>
+      <c r="C24" t="s">
+        <v>380</v>
+      </c>
       <c r="F24" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
+      <c r="B25" t="s">
+        <v>381</v>
+      </c>
+      <c r="C25" t="s">
+        <v>382</v>
+      </c>
       <c r="F25" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>51</v>
       </c>
+      <c r="B26" t="s">
+        <v>383</v>
+      </c>
+      <c r="C26" t="s">
+        <v>384</v>
+      </c>
       <c r="F26" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>53</v>
       </c>
+      <c r="C27" t="s">
+        <v>352</v>
+      </c>
       <c r="F27" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>55</v>
       </c>
+      <c r="B28" t="s">
+        <v>385</v>
+      </c>
+      <c r="C28" t="s">
+        <v>386</v>
+      </c>
       <c r="F28" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>57</v>
       </c>
+      <c r="B29" t="s">
+        <v>387</v>
+      </c>
+      <c r="C29" t="s">
+        <v>388</v>
+      </c>
       <c r="F29" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>59</v>
       </c>
+      <c r="B30" t="s">
+        <v>389</v>
+      </c>
+      <c r="C30" t="s">
+        <v>390</v>
+      </c>
       <c r="F30" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>61</v>
       </c>
+      <c r="B31" t="s">
+        <v>391</v>
+      </c>
+      <c r="C31" t="s">
+        <v>392</v>
+      </c>
       <c r="F31" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>62</v>
       </c>
+      <c r="C32" t="s">
+        <v>352</v>
+      </c>
       <c r="F32" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>64</v>
       </c>
+      <c r="C33" t="s">
+        <v>352</v>
+      </c>
       <c r="F33" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>66</v>
       </c>
+      <c r="D34" t="s">
+        <v>361</v>
+      </c>
       <c r="F34" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>68</v>
       </c>
+      <c r="B35" t="s">
+        <v>368</v>
+      </c>
+      <c r="C35" t="s">
+        <v>369</v>
+      </c>
       <c r="F35" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>70</v>
       </c>
+      <c r="B36" t="s">
+        <v>393</v>
+      </c>
+      <c r="C36" t="s">
+        <v>394</v>
+      </c>
       <c r="F36" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
+      <c r="B37" t="s">
+        <v>393</v>
+      </c>
+      <c r="C37" t="s">
+        <v>394</v>
+      </c>
       <c r="F37" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
+      <c r="D38" t="s">
+        <v>361</v>
+      </c>
       <c r="F38" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>76</v>
       </c>
+      <c r="C39" t="s">
+        <v>352</v>
+      </c>
       <c r="F39" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>77</v>
       </c>
+      <c r="B40" t="s">
+        <v>359</v>
+      </c>
+      <c r="C40" t="s">
+        <v>360</v>
+      </c>
       <c r="F40" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>79</v>
       </c>
+      <c r="B41" t="s">
+        <v>353</v>
+      </c>
+      <c r="C41" t="s">
+        <v>354</v>
+      </c>
       <c r="F41" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>81</v>
       </c>
+      <c r="B42" t="s">
+        <v>395</v>
+      </c>
+      <c r="C42" t="s">
+        <v>396</v>
+      </c>
       <c r="F42" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>83</v>
       </c>
+      <c r="D43" t="s">
+        <v>361</v>
+      </c>
       <c r="F43" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>85</v>
       </c>
+      <c r="C44" t="s">
+        <v>352</v>
+      </c>
       <c r="F44" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>87</v>
       </c>
+      <c r="D45" t="s">
+        <v>361</v>
+      </c>
       <c r="F45" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>89</v>
       </c>
+      <c r="B46" t="s">
+        <v>397</v>
+      </c>
+      <c r="C46" t="s">
+        <v>398</v>
+      </c>
       <c r="F46" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>91</v>
       </c>
+      <c r="C47" t="s">
+        <v>352</v>
+      </c>
       <c r="F47" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="C48" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="C49" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="B50" t="s">
+        <v>399</v>
+      </c>
+      <c r="C50" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="B51" t="s">
+        <v>366</v>
+      </c>
+      <c r="C51" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="C52" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="C53" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="B54" t="s">
+        <v>353</v>
+      </c>
+      <c r="C54" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="B55" t="s">
+        <v>391</v>
+      </c>
+      <c r="C55" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="B56" t="s">
+        <v>366</v>
+      </c>
+      <c r="C56" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="B57" t="s">
+        <v>391</v>
+      </c>
+      <c r="C57" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="B58" t="s">
+        <v>391</v>
+      </c>
+      <c r="C58" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="B59" t="s">
+        <v>401</v>
+      </c>
+      <c r="C59" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="B60" t="s">
+        <v>403</v>
+      </c>
+      <c r="C60" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="B61" t="s">
+        <v>405</v>
+      </c>
+      <c r="C61" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="B62" t="s">
+        <v>359</v>
+      </c>
+      <c r="C62" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="B63" t="s">
+        <v>397</v>
+      </c>
+      <c r="C63" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="B64" t="s">
+        <v>407</v>
+      </c>
+      <c r="C64" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="C65" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="C66" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="B67" t="s">
+        <v>357</v>
+      </c>
+      <c r="C67" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="B68" t="s">
+        <v>409</v>
+      </c>
+      <c r="C68" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="C69" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="C70" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="B71" t="s">
+        <v>411</v>
+      </c>
+      <c r="C71" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="B72" t="s">
+        <v>366</v>
+      </c>
+      <c r="C72" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="B73" t="s">
+        <v>413</v>
+      </c>
+      <c r="C73" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="B74" t="s">
+        <v>415</v>
+      </c>
+      <c r="C74" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="B75" t="s">
+        <v>417</v>
+      </c>
+      <c r="C75" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="B76" t="s">
+        <v>366</v>
+      </c>
+      <c r="C76" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="D77" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="B78" t="s">
+        <v>403</v>
+      </c>
+      <c r="C78" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="B79" t="s">
+        <v>419</v>
+      </c>
+      <c r="C79" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="B80" t="s">
+        <v>421</v>
+      </c>
+      <c r="C80" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="B81" t="s">
+        <v>423</v>
+      </c>
+      <c r="C81" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="B82" t="s">
+        <v>355</v>
+      </c>
+      <c r="C82" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="B83" t="s">
+        <v>425</v>
+      </c>
+      <c r="C83" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="C84" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="B85" t="s">
+        <v>389</v>
+      </c>
+      <c r="C85" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="B86" t="s">
+        <v>427</v>
+      </c>
+      <c r="C86" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="B87" t="s">
+        <v>429</v>
+      </c>
+      <c r="C87" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="B88" t="s">
+        <v>425</v>
+      </c>
+      <c r="C88" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="B89" t="s">
+        <v>431</v>
+      </c>
+      <c r="C89" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="B90" t="s">
+        <v>391</v>
+      </c>
+      <c r="C90" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="B91" t="s">
+        <v>393</v>
+      </c>
+      <c r="C91" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="B92" t="s">
+        <v>433</v>
+      </c>
+      <c r="C92" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="B93" t="s">
+        <v>419</v>
+      </c>
+      <c r="C93" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="C94" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="B95" t="s">
+        <v>86</v>
+      </c>
+      <c r="C95" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="C96" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="B97" t="s">
+        <v>435</v>
+      </c>
+      <c r="C97" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="B98" t="s">
+        <v>427</v>
+      </c>
+      <c r="C98" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="B99" t="s">
+        <v>86</v>
+      </c>
+      <c r="C99" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="B100" t="s">
+        <v>421</v>
+      </c>
+      <c r="C100" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="B101" t="s">
+        <v>427</v>
+      </c>
+      <c r="C101" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="B102" t="s">
+        <v>437</v>
+      </c>
+      <c r="C102" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="B103" t="s">
+        <v>383</v>
+      </c>
+      <c r="C103" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="D104" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="B105" t="s">
+        <v>370</v>
+      </c>
+      <c r="C105" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="B106" t="s">
+        <v>391</v>
+      </c>
+      <c r="C106" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="B107" t="s">
+        <v>391</v>
+      </c>
+      <c r="C107" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="B108" t="s">
+        <v>391</v>
+      </c>
+      <c r="C108" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="B109" t="s">
+        <v>391</v>
+      </c>
+      <c r="C109" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="B110" t="s">
+        <v>391</v>
+      </c>
+      <c r="C110" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="B111" t="s">
+        <v>391</v>
+      </c>
+      <c r="C111" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="B112" t="s">
+        <v>391</v>
+      </c>
+      <c r="C112" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="B113" t="s">
+        <v>391</v>
+      </c>
+      <c r="C113" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="115" spans="1:6">
+      <c r="B114" t="s">
+        <v>391</v>
+      </c>
+      <c r="C114" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="B115" t="s">
+        <v>366</v>
+      </c>
+      <c r="C115" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="B116" t="s">
+        <v>393</v>
+      </c>
+      <c r="C116" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="D117" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="B118" t="s">
+        <v>439</v>
+      </c>
+      <c r="C118" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="120" spans="1:6">
+      <c r="B119" t="s">
+        <v>411</v>
+      </c>
+      <c r="C119" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="B120" t="s">
+        <v>353</v>
+      </c>
+      <c r="C120" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
+      <c r="B121" t="s">
+        <v>364</v>
+      </c>
+      <c r="C121" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="D122" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="D123" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="D124" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="126" spans="1:6">
+      <c r="B125" t="s">
+        <v>391</v>
+      </c>
+      <c r="C125" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="127" spans="1:6">
+      <c r="B126" t="s">
+        <v>395</v>
+      </c>
+      <c r="C126" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="B127" t="s">
+        <v>359</v>
+      </c>
+      <c r="C127" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="B128" t="s">
+        <v>433</v>
+      </c>
+      <c r="C128" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="130" spans="1:6">
+      <c r="C129" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="C130" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="C131" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="133" spans="1:6">
+      <c r="D132" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="B133" t="s">
+        <v>391</v>
+      </c>
+      <c r="C133" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="135" spans="1:6">
+      <c r="B134" t="s">
+        <v>441</v>
+      </c>
+      <c r="C134" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="136" spans="1:6">
+      <c r="D135" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="137" spans="1:6">
+      <c r="C136" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="138" spans="1:6">
+      <c r="B137" t="s">
+        <v>443</v>
+      </c>
+      <c r="C137" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="139" spans="1:6">
+      <c r="B138" t="s">
+        <v>445</v>
+      </c>
+      <c r="C138" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="140" spans="1:6">
+      <c r="B139" t="s">
+        <v>366</v>
+      </c>
+      <c r="C139" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="141" spans="1:6">
+      <c r="B140" t="s">
+        <v>353</v>
+      </c>
+      <c r="C140" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="142" spans="1:6">
+      <c r="C141" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="143" spans="1:6">
+      <c r="B142" t="s">
+        <v>366</v>
+      </c>
+      <c r="C142" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="144" spans="1:6">
+      <c r="B143" t="s">
+        <v>370</v>
+      </c>
+      <c r="C143" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="D144" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="146" spans="1:6">
+      <c r="B145" t="s">
+        <v>389</v>
+      </c>
+      <c r="C145" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="147" spans="1:6">
+      <c r="B146" t="s">
+        <v>447</v>
+      </c>
+      <c r="C146" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="148" spans="1:6">
+      <c r="B147" t="s">
+        <v>449</v>
+      </c>
+      <c r="C147" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="149" spans="1:6">
+      <c r="B148" t="s">
+        <v>451</v>
+      </c>
+      <c r="C148" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="D149" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="151" spans="1:6">
+      <c r="B150" t="s">
+        <v>453</v>
+      </c>
+      <c r="C150" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="152" spans="1:6">
+      <c r="D151" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="153" spans="1:6">
+      <c r="B152" t="s">
+        <v>86</v>
+      </c>
+      <c r="C152" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="154" spans="1:6">
+      <c r="B153" t="s">
+        <v>359</v>
+      </c>
+      <c r="C153" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="155" spans="1:6">
+      <c r="B154" t="s">
+        <v>383</v>
+      </c>
+      <c r="C154" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="156" spans="1:6">
+      <c r="B155" t="s">
+        <v>447</v>
+      </c>
+      <c r="C155" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="157" spans="1:6">
+      <c r="B156" t="s">
+        <v>421</v>
+      </c>
+      <c r="C156" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="158" spans="1:6">
+      <c r="C157" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="159" spans="1:6">
+      <c r="B158" t="s">
+        <v>391</v>
+      </c>
+      <c r="C158" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="160" spans="1:6">
+      <c r="C159" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="161" spans="1:6">
+      <c r="B160" t="s">
+        <v>387</v>
+      </c>
+      <c r="C160" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="162" spans="1:6">
+      <c r="B161" t="s">
+        <v>374</v>
+      </c>
+      <c r="C161" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="163" spans="1:6">
+      <c r="B162" t="s">
+        <v>443</v>
+      </c>
+      <c r="C162" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="164" spans="1:6">
+      <c r="B163" t="s">
+        <v>455</v>
+      </c>
+      <c r="C163" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="165" spans="1:6">
+      <c r="B164" t="s">
+        <v>457</v>
+      </c>
+      <c r="C164" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="166" spans="1:6">
+      <c r="D165" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="167" spans="1:6">
+      <c r="B166" t="s">
+        <v>370</v>
+      </c>
+      <c r="C166" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="168" spans="1:6">
+      <c r="B167" t="s">
+        <v>423</v>
+      </c>
+      <c r="C167" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="169" spans="1:6">
+      <c r="B168" t="s">
+        <v>459</v>
+      </c>
+      <c r="C168" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="170" spans="1:6">
+      <c r="D169" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="171" spans="1:6">
+      <c r="D170" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="172" spans="1:6">
+      <c r="B171" t="s">
+        <v>427</v>
+      </c>
+      <c r="C171" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="173" spans="1:6">
+      <c r="B172" t="s">
+        <v>391</v>
+      </c>
+      <c r="C172" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="174" spans="1:6">
+      <c r="B173" t="s">
+        <v>461</v>
+      </c>
+      <c r="C173" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="175" spans="1:6">
+      <c r="B174" t="s">
+        <v>405</v>
+      </c>
+      <c r="C174" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="176" spans="1:6">
+      <c r="B175" t="s">
+        <v>425</v>
+      </c>
+      <c r="C175" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="177" spans="1:6">
+      <c r="B176" t="s">
+        <v>463</v>
+      </c>
+      <c r="C176" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="178" spans="1:6">
+      <c r="D177" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="179" spans="1:6">
+      <c r="B178" t="s">
+        <v>12</v>
+      </c>
+      <c r="C178" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="180" spans="1:6">
+      <c r="D179" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="181" spans="1:6">
+      <c r="C180" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="182" spans="1:6">
+      <c r="C181" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="183" spans="1:6">
+      <c r="B182" t="s">
+        <v>455</v>
+      </c>
+      <c r="C182" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="184" spans="1:6">
+      <c r="B183" t="s">
+        <v>451</v>
+      </c>
+      <c r="C183" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="185" spans="1:6">
+      <c r="B184" t="s">
+        <v>466</v>
+      </c>
+      <c r="C184" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="186" spans="1:6">
+      <c r="C185" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="187" spans="1:6">
+      <c r="B186" t="s">
+        <v>443</v>
+      </c>
+      <c r="C186" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="188" spans="1:6">
+      <c r="C187" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="189" spans="1:6">
+      <c r="B188" t="s">
+        <v>468</v>
+      </c>
+      <c r="C188" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="190" spans="1:6">
+      <c r="B189" t="s">
+        <v>391</v>
+      </c>
+      <c r="C189" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="191" spans="1:6">
+      <c r="B190" t="s">
+        <v>397</v>
+      </c>
+      <c r="C190" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="192" spans="1:6">
+      <c r="B191" t="s">
+        <v>470</v>
+      </c>
+      <c r="C191" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="193" spans="1:6">
+      <c r="D192" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="194" spans="1:6">
+      <c r="C193" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="195" spans="1:6">
+      <c r="B194" t="s">
+        <v>472</v>
+      </c>
+      <c r="C194" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="196" spans="1:6">
+      <c r="B195" t="s">
+        <v>474</v>
+      </c>
+      <c r="C195" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="197" spans="1:6">
+      <c r="B196" t="s">
+        <v>433</v>
+      </c>
+      <c r="C196" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="198" spans="1:6">
+      <c r="C197" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="199" spans="1:6">
+      <c r="B198" t="s">
+        <v>403</v>
+      </c>
+      <c r="C198" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="200" spans="1:6">
+      <c r="B199" t="s">
+        <v>476</v>
+      </c>
+      <c r="C199" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="201" spans="1:6">
+      <c r="B200" t="s">
+        <v>407</v>
+      </c>
+      <c r="C200" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="202" spans="1:6">
+      <c r="C201" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="203" spans="1:6">
+      <c r="C202" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="204" spans="1:6">
+      <c r="B203" t="s">
+        <v>407</v>
+      </c>
+      <c r="C203" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="205" spans="1:6">
+      <c r="B204" t="s">
+        <v>443</v>
+      </c>
+      <c r="C204" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="206" spans="1:6">
+      <c r="C205" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="207" spans="1:6">
+      <c r="B206" t="s">
+        <v>368</v>
+      </c>
+      <c r="C206" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="208" spans="1:6">
+      <c r="B207" t="s">
+        <v>353</v>
+      </c>
+      <c r="C207" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="209" spans="1:6">
+      <c r="D208" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="210" spans="1:6">
+      <c r="B209" t="s">
+        <v>397</v>
+      </c>
+      <c r="C209" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="211" spans="1:6">
+      <c r="C210" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="212" spans="1:6">
+      <c r="B211" t="s">
+        <v>353</v>
+      </c>
+      <c r="C211" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="213" spans="1:6">
+      <c r="B212" t="s">
+        <v>366</v>
+      </c>
+      <c r="C212" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="214" spans="1:6">
+      <c r="B213" t="s">
+        <v>370</v>
+      </c>
+      <c r="C213" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="215" spans="1:6">
+      <c r="B214" t="s">
+        <v>427</v>
+      </c>
+      <c r="C214" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="216" spans="1:6">
+      <c r="B215" t="s">
+        <v>383</v>
+      </c>
+      <c r="C215" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="217" spans="1:6">
+      <c r="B216" t="s">
+        <v>478</v>
+      </c>
+      <c r="C216" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="218" spans="1:6">
+      <c r="D217" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="219" spans="1:6">
+      <c r="B218" t="s">
+        <v>447</v>
+      </c>
+      <c r="C218" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="220" spans="1:6">
+      <c r="C219" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="221" spans="1:6">
+      <c r="B220" t="s">
+        <v>480</v>
+      </c>
+      <c r="C220" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="222" spans="1:6">
+      <c r="B221" t="s">
+        <v>482</v>
+      </c>
+      <c r="C221" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="223" spans="1:6">
+      <c r="B222" t="s">
+        <v>484</v>
+      </c>
+      <c r="C222" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="224" spans="1:6">
+      <c r="C223" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="225" spans="1:6">
+      <c r="B224" t="s">
+        <v>391</v>
+      </c>
+      <c r="C224" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="226" spans="1:6">
+      <c r="B225" t="s">
+        <v>389</v>
+      </c>
+      <c r="C225" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="227" spans="1:6">
+      <c r="C226" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="228" spans="1:6">
+      <c r="B227" t="s">
+        <v>393</v>
+      </c>
+      <c r="C227" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="229" spans="1:6">
+      <c r="C228" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="230" spans="1:6">
+      <c r="D229" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="231" spans="1:6">
+      <c r="B230" t="s">
+        <v>368</v>
+      </c>
+      <c r="C230" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="232" spans="1:6">
+      <c r="C231" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="233" spans="1:6">
+      <c r="B232" t="s">
+        <v>366</v>
+      </c>
+      <c r="C232" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="234" spans="1:6">
+      <c r="B233" t="s">
+        <v>413</v>
+      </c>
+      <c r="C233" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="235" spans="1:6">
+      <c r="D234" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="236" spans="1:6">
+      <c r="B235" t="s">
+        <v>427</v>
+      </c>
+      <c r="C235" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="237" spans="1:6">
+      <c r="B236" t="s">
+        <v>413</v>
+      </c>
+      <c r="C236" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="238" spans="1:6">
+      <c r="B237" t="s">
+        <v>407</v>
+      </c>
+      <c r="C237" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="239" spans="1:6">
+      <c r="B238" t="s">
+        <v>391</v>
+      </c>
+      <c r="C238" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="240" spans="1:6">
+      <c r="B239" t="s">
+        <v>366</v>
+      </c>
+      <c r="C239" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="241" spans="1:6">
+      <c r="B240" t="s">
+        <v>366</v>
+      </c>
+      <c r="C240" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="242" spans="1:6">
+      <c r="B241" t="s">
+        <v>407</v>
+      </c>
+      <c r="C241" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="243" spans="1:6">
+      <c r="B242" t="s">
+        <v>486</v>
+      </c>
+      <c r="C242" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="244" spans="1:6">
+      <c r="B243" t="s">
+        <v>366</v>
+      </c>
+      <c r="C243" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="245" spans="1:6">
+      <c r="B244" t="s">
+        <v>447</v>
+      </c>
+      <c r="C244" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="246" spans="1:6">
+      <c r="B245" t="s">
+        <v>86</v>
+      </c>
+      <c r="C245" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="247" spans="1:6">
+      <c r="B246" t="s">
+        <v>488</v>
+      </c>
+      <c r="C246" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="248" spans="1:6">
+      <c r="B247" t="s">
+        <v>443</v>
+      </c>
+      <c r="C247" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="249" spans="1:6">
+      <c r="B248" t="s">
+        <v>443</v>
+      </c>
+      <c r="C248" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="250" spans="1:6">
+      <c r="B249" t="s">
+        <v>443</v>
+      </c>
+      <c r="C249" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="251" spans="1:6">
+      <c r="B250" t="s">
+        <v>366</v>
+      </c>
+      <c r="C250" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="252" spans="1:6">
+      <c r="B251" t="s">
+        <v>370</v>
+      </c>
+      <c r="C251" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="253" spans="1:6">
+      <c r="D252" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="254" spans="1:6">
+      <c r="B253" t="s">
+        <v>86</v>
+      </c>
+      <c r="C253" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="255" spans="1:6">
+      <c r="B254" t="s">
+        <v>383</v>
+      </c>
+      <c r="C254" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="256" spans="1:6">
+      <c r="B255" t="s">
+        <v>393</v>
+      </c>
+      <c r="C255" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="257" spans="1:6">
+      <c r="D256" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="258" spans="1:6">
+      <c r="C257" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="259" spans="1:6">
+      <c r="B258" t="s">
+        <v>490</v>
+      </c>
+      <c r="C258" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="260" spans="1:6">
+      <c r="C259" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="261" spans="1:6">
+      <c r="B260" t="s">
+        <v>12</v>
+      </c>
+      <c r="C260" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="262" spans="1:6">
+      <c r="C261" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="263" spans="1:6">
+      <c r="B262" t="s">
+        <v>459</v>
+      </c>
+      <c r="C262" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="264" spans="1:6">
+      <c r="C263" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="265" spans="1:6">
+      <c r="B264" t="s">
+        <v>366</v>
+      </c>
+      <c r="C264" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="266" spans="1:6">
+      <c r="B265" t="s">
+        <v>387</v>
+      </c>
+      <c r="C265" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="267" spans="1:6">
+      <c r="C266" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="268" spans="1:6">
+      <c r="D267" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="269" spans="1:6">
+      <c r="B268" t="s">
+        <v>359</v>
+      </c>
+      <c r="C268" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="270" spans="1:6">
+      <c r="B269" t="s">
+        <v>474</v>
+      </c>
+      <c r="C269" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="271" spans="1:6">
+      <c r="B270" t="s">
+        <v>492</v>
+      </c>
+      <c r="C270" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="272" spans="1:6">
+      <c r="C271" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="273" spans="1:6">
+      <c r="B272" t="s">
+        <v>494</v>
+      </c>
+      <c r="C272" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="274" spans="1:6">
+      <c r="C273" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="275" spans="1:6">
+      <c r="B274" t="s">
+        <v>364</v>
+      </c>
+      <c r="C274" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="276" spans="1:6">
+      <c r="B275" t="s">
+        <v>437</v>
+      </c>
+      <c r="C275" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="277" spans="1:6">
+      <c r="B276" t="s">
+        <v>374</v>
+      </c>
+      <c r="C276" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="278" spans="1:6">
+      <c r="C277" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="279" spans="1:6">
+      <c r="C278" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="280" spans="1:6">
+      <c r="B279" t="s">
+        <v>397</v>
+      </c>
+      <c r="C279" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="281" spans="1:6">
+      <c r="D280" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="282" spans="1:6">
+      <c r="B281" t="s">
+        <v>433</v>
+      </c>
+      <c r="C281" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="283" spans="1:6">
+      <c r="B282" t="s">
+        <v>393</v>
+      </c>
+      <c r="C282" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="284" spans="1:6">
+      <c r="B283" t="s">
+        <v>366</v>
+      </c>
+      <c r="C283" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="285" spans="1:6">
+      <c r="C284" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="286" spans="1:6">
+      <c r="D285" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="287" spans="1:6">
+      <c r="D286" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="288" spans="1:6">
+      <c r="D287" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="289" spans="1:6">
+      <c r="B288" t="s">
+        <v>6</v>
+      </c>
+      <c r="C288" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="290" spans="1:6">
+      <c r="B289" t="s">
+        <v>427</v>
+      </c>
+      <c r="C289" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="291" spans="1:6">
+      <c r="C290" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="292" spans="1:6">
+      <c r="B291" t="s">
+        <v>370</v>
+      </c>
+      <c r="C291" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="293" spans="1:6">
+      <c r="B292" t="s">
+        <v>353</v>
+      </c>
+      <c r="C292" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="294" spans="1:6">
+      <c r="C293" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="295" spans="1:6">
+      <c r="B294" t="s">
+        <v>12</v>
+      </c>
+      <c r="C294" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="296" spans="1:6">
+      <c r="D295" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="297" spans="1:6">
+      <c r="B296" t="s">
+        <v>496</v>
+      </c>
+      <c r="C296" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="298" spans="1:6">
+      <c r="C297" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="299" spans="1:6">
+      <c r="B298" t="s">
+        <v>6</v>
+      </c>
+      <c r="C298" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="300" spans="1:6">
+      <c r="C299" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="301" spans="1:6">
+      <c r="B300" t="s">
+        <v>383</v>
+      </c>
+      <c r="C300" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="302" spans="1:6">
+      <c r="D301" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="303" spans="1:6">
+      <c r="C302" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="304" spans="1:6">
+      <c r="B303" t="s">
+        <v>353</v>
+      </c>
+      <c r="C303" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="305" spans="1:6">
+      <c r="C304" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="306" spans="1:6">
+      <c r="C305" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="307" spans="1:6">
+      <c r="D306" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>351</v>
       </c>
+      <c r="B307" t="s">
+        <v>461</v>
+      </c>
+      <c r="C307" t="s">
+        <v>462</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <autoFilter ref="A1:D307" xr:uid="{619B19FF-0082-0E4F-A35B-9ACBD206B038}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>